<commit_message>
Big changes in chapter 6. Testing.
</commit_message>
<xml_diff>
--- a/docs/AnalysisData/MarkerContentTests.xlsx
+++ b/docs/AnalysisData/MarkerContentTests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="13395" windowHeight="5190" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="13395" windowHeight="5190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Text Normal" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
   <si>
     <t>1 marker</t>
   </si>
@@ -44,13 +44,24 @@
   <si>
     <t>max</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -106,6 +117,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +434,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:I9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" ref="E9:I9" si="5">MAX(G3:G7)</f>
+        <f t="shared" ref="G9:I9" si="5">MAX(G3:G7)</f>
         <v>91.198700000000002</v>
       </c>
       <c r="H9" s="7">
@@ -646,9 +670,37 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>1.3730189638165964</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:I10" si="6">_xlfn.STDEV.S(C3:C7)</f>
+        <v>1.6558614757883543</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="6"/>
+        <v>2.1287612670283136</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.5661750497858431</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="6"/>
+        <v>1.7641168960701006</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="6"/>
+        <v>3.4337766492595305</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
@@ -699,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,12 +1001,36 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>1.3974466519334425</v>
+      </c>
+      <c r="C10" s="18">
+        <f t="shared" ref="C10:D10" si="4">_xlfn.STDEV.S(C3:C7)</f>
+        <v>2.2026716573288918</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="4"/>
+        <v>3.4012010415440024</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="18">
+        <f>_xlfn.STDEV.S(G3:G7)</f>
+        <v>2.344629258966116</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10:I10" si="5">_xlfn.STDEV.S(H3:H7)</f>
+        <v>2.7949021571425363</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="5"/>
+        <v>3.9558313357624333</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
@@ -1014,7 +1090,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,12 +1360,37 @@
       <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>0.36907135218003784</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" ref="C10:D10" si="4">_xlfn.STDEV.S(C3:C7)</f>
+        <v>0.33219781757260142</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="4"/>
+        <v>1.3052635741489123</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="18">
+        <f>_xlfn.STDEV.S(G3:G7)</f>
+        <v>0.46407015956641889</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10:I10" si="5">_xlfn.STDEV.S(H3:H7)</f>
+        <v>0.40131540214649086</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="5"/>
+        <v>1.3197916608313589</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1403,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,6 +1755,38 @@
         <v>93.337699999999998</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>1.3378074386846577</v>
+      </c>
+      <c r="C10" s="18">
+        <f t="shared" ref="C10:D10" si="4">_xlfn.STDEV.S(C3:C7)</f>
+        <v>1.0024264227363491</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="4"/>
+        <v>2.0177661497309356</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="18">
+        <f>_xlfn.STDEV.S(G3:G7)</f>
+        <v>0.46645910538866969</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10:I10" si="5">_xlfn.STDEV.S(H3:H7)</f>
+        <v>0.37021579923066178</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="5"/>
+        <v>0.93236083787340251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1661,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="A1:I9"/>
+      <selection activeCell="D10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,76 +1848,136 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="15">
+        <v>75.272099999999995</v>
+      </c>
+      <c r="C3" s="15">
+        <v>77.118799999999993</v>
+      </c>
+      <c r="D3" s="15">
+        <v>62.139000000000003</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12">
         <v>1</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="G3" s="16">
+        <v>86.338099999999997</v>
+      </c>
+      <c r="H3" s="16">
+        <v>79.976500000000001</v>
+      </c>
+      <c r="I3" s="16">
+        <v>81.441900000000004</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="15">
+        <v>74.249799999999993</v>
+      </c>
+      <c r="C4" s="15">
+        <v>78.030100000000004</v>
+      </c>
+      <c r="D4" s="15">
+        <v>69.262100000000004</v>
+      </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="16">
+        <v>86.168300000000002</v>
+      </c>
+      <c r="H4" s="16">
+        <v>81.210700000000003</v>
+      </c>
+      <c r="I4" s="16">
+        <v>84.132000000000005</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="15">
+        <v>72.9298</v>
+      </c>
+      <c r="C5" s="15">
+        <v>78.341800000000006</v>
+      </c>
+      <c r="D5" s="15">
+        <v>62.021000000000001</v>
+      </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="16">
+        <v>86.566299999999998</v>
+      </c>
+      <c r="H5" s="16">
+        <v>81.255600000000001</v>
+      </c>
+      <c r="I5" s="16">
+        <v>83.118399999999994</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="15">
+        <v>72.253200000000007</v>
+      </c>
+      <c r="C6" s="15">
+        <v>78.034899999999993</v>
+      </c>
+      <c r="D6" s="15">
+        <v>60.930599999999998</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="16">
+        <v>86.942899999999995</v>
+      </c>
+      <c r="H6" s="16">
+        <v>80.981999999999999</v>
+      </c>
+      <c r="I6" s="16">
+        <v>80.459500000000006</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="15">
+        <v>74.743200000000002</v>
+      </c>
+      <c r="C7" s="15">
+        <v>79.106700000000004</v>
+      </c>
+      <c r="D7" s="15">
+        <v>63.543900000000001</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="16">
+        <v>87.163899999999998</v>
+      </c>
+      <c r="H7" s="16">
+        <v>81.0608</v>
+      </c>
+      <c r="I7" s="16">
+        <v>82.159000000000006</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -1792,15 +1985,15 @@
       </c>
       <c r="B8" s="13">
         <f>MIN(B3:B7)</f>
-        <v>0</v>
+        <v>72.253200000000007</v>
       </c>
       <c r="C8" s="13">
         <f t="shared" ref="C8:D8" si="0">MIN(C3:C7)</f>
-        <v>0</v>
+        <v>77.118799999999993</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.930599999999998</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
@@ -1808,15 +2001,15 @@
       </c>
       <c r="G8" s="3">
         <f>MIN(G3:G7)</f>
-        <v>0</v>
+        <v>86.168300000000002</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" ref="H8:I8" si="1">MIN(H3:H7)</f>
-        <v>0</v>
+        <v>79.976500000000001</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80.459500000000006</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1825,15 +2018,15 @@
       </c>
       <c r="B9" s="13">
         <f>MAX(B3:B7)</f>
-        <v>0</v>
+        <v>75.272099999999995</v>
       </c>
       <c r="C9" s="13">
         <f t="shared" ref="C9:D9" si="2">MAX(C3:C7)</f>
-        <v>0</v>
+        <v>79.106700000000004</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>69.262100000000004</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
@@ -1841,15 +2034,47 @@
       </c>
       <c r="G9" s="3">
         <f>MAX(G3:G7)</f>
-        <v>0</v>
+        <v>87.163899999999998</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" ref="H9:I9" si="3">MAX(H3:H7)</f>
-        <v>0</v>
+        <v>81.255600000000001</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>84.132000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>1.2618145909760239</v>
+      </c>
+      <c r="C10" s="18">
+        <f t="shared" ref="C10:D10" si="4">_xlfn.STDEV.S(C3:C7)</f>
+        <v>0.71419341427935756</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="4"/>
+        <v>3.30960132296928</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="18">
+        <f>_xlfn.STDEV.S(G3:G7)</f>
+        <v>0.41388759343570408</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10:I10" si="5">_xlfn.STDEV.S(H3:H7)</f>
+        <v>0.52639748954568544</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="5"/>
+        <v>1.4285044707665409</v>
       </c>
     </row>
   </sheetData>
@@ -1859,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I9"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,76 +2138,136 @@
       <c r="A3" s="12">
         <v>1</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="17">
+        <v>42.412100000000002</v>
+      </c>
+      <c r="C3" s="17">
+        <v>36.2301</v>
+      </c>
+      <c r="D3" s="17">
+        <v>5.8418100000000006</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12">
         <v>1</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="G3" s="18">
+        <v>89.274799999999999</v>
+      </c>
+      <c r="H3" s="18">
+        <v>76.346599999999995</v>
+      </c>
+      <c r="I3" s="18">
+        <v>79.730999999999995</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="17">
+        <v>42.624899999999997</v>
+      </c>
+      <c r="C4" s="17">
+        <v>32.069500000000005</v>
+      </c>
+      <c r="D4" s="17">
+        <v>3.3645959999999997</v>
+      </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="G4" s="18">
+        <v>87.763800000000003</v>
+      </c>
+      <c r="H4" s="18">
+        <v>68.956100000000006</v>
+      </c>
+      <c r="I4" s="18">
+        <v>74.397000000000006</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="B5" s="17">
+        <v>42.591900000000003</v>
+      </c>
+      <c r="C5" s="17">
+        <v>36.211599999999997</v>
+      </c>
+      <c r="D5" s="17">
+        <v>3.75759</v>
+      </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12">
         <v>3</v>
       </c>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="18">
+        <v>87.2286</v>
+      </c>
+      <c r="H5" s="18">
+        <v>71.222800000000007</v>
+      </c>
+      <c r="I5" s="18">
+        <v>74.981499999999997</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="17">
+        <v>42.526299999999999</v>
+      </c>
+      <c r="C6" s="17">
+        <v>37.657200000000003</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3.3313600000000001</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12">
         <v>4</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="18">
+        <v>88.888499999999993</v>
+      </c>
+      <c r="H6" s="18">
+        <v>70.728499999999997</v>
+      </c>
+      <c r="I6" s="18">
+        <v>80.046899999999994</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="17">
+        <v>43.695300000000003</v>
+      </c>
+      <c r="C7" s="17">
+        <v>37.285299999999999</v>
+      </c>
+      <c r="D7" s="17">
+        <v>5.3274900000000001</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12">
         <v>5</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="18">
+        <v>88.773600000000002</v>
+      </c>
+      <c r="H7" s="18">
+        <v>73.440299999999993</v>
+      </c>
+      <c r="I7" s="18">
+        <v>81.162599999999998</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -1990,15 +2275,15 @@
       </c>
       <c r="B8" s="13">
         <f>MIN(B3:B7)</f>
-        <v>0</v>
+        <v>42.412100000000002</v>
       </c>
       <c r="C8" s="13">
         <f t="shared" ref="C8:D8" si="0">MIN(C3:C7)</f>
-        <v>0</v>
+        <v>32.069500000000005</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3313600000000001</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
@@ -2006,15 +2291,15 @@
       </c>
       <c r="G8" s="3">
         <f>MIN(G3:G7)</f>
-        <v>0</v>
+        <v>87.2286</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" ref="H8:I8" si="1">MIN(H3:H7)</f>
-        <v>0</v>
+        <v>68.956100000000006</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>74.397000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2023,15 +2308,15 @@
       </c>
       <c r="B9" s="13">
         <f>MAX(B3:B7)</f>
-        <v>0</v>
+        <v>43.695300000000003</v>
       </c>
       <c r="C9" s="13">
         <f t="shared" ref="C9:D9" si="2">MAX(C3:C7)</f>
-        <v>0</v>
+        <v>37.657200000000003</v>
       </c>
       <c r="D9" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.8418100000000006</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
@@ -2039,15 +2324,47 @@
       </c>
       <c r="G9" s="3">
         <f>MAX(G3:G7)</f>
-        <v>0</v>
+        <v>89.274799999999999</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" ref="H9:I9" si="3">MAX(H3:H7)</f>
-        <v>0</v>
+        <v>76.346599999999995</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>81.162599999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="18">
+        <f>_xlfn.STDEV.S(B3:B7)</f>
+        <v>0.52355414237689035</v>
+      </c>
+      <c r="C10" s="18">
+        <f t="shared" ref="C10:D10" si="4">_xlfn.STDEV.S(C3:C7)</f>
+        <v>2.2296395455319664</v>
+      </c>
+      <c r="D10" s="18">
+        <f t="shared" si="4"/>
+        <v>1.1765785406394247</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="18">
+        <f>_xlfn.STDEV.S(G3:G7)</f>
+        <v>0.85431448425038259</v>
+      </c>
+      <c r="H10" s="18">
+        <f t="shared" ref="H10:I10" si="5">_xlfn.STDEV.S(H3:H7)</f>
+        <v>2.8441635172753301</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="5"/>
+        <v>3.1329218957707803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>